<commit_message>
added fci documents and edited physics es document
</commit_message>
<xml_diff>
--- a/primo anno/fisica modulo 1/esercizi fisica eserciziario.xlsx
+++ b/primo anno/fisica modulo 1/esercizi fisica eserciziario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomma\Documents\uni\primo anno\fisica modulo 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F216917-1EF2-4859-8CCA-AF8FC8C94B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CB0833-97FE-44B6-A94F-962AD9EC5525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C46B4579-7AB7-47FB-BF5E-61A492D5042E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C46B4579-7AB7-47FB-BF5E-61A492D5042E}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="127">
   <si>
     <t>cinematica</t>
   </si>
@@ -244,6 +244,168 @@
   </si>
   <si>
     <t>4.22</t>
+  </si>
+  <si>
+    <t>corpo rigido e gravitazione</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>5.8</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>5.10</t>
+  </si>
+  <si>
+    <t>5.11</t>
+  </si>
+  <si>
+    <t>5.12</t>
+  </si>
+  <si>
+    <t>5.13</t>
+  </si>
+  <si>
+    <t>5.14</t>
+  </si>
+  <si>
+    <t>5.15</t>
+  </si>
+  <si>
+    <t>5.16</t>
+  </si>
+  <si>
+    <t>5.17</t>
+  </si>
+  <si>
+    <t>5.18</t>
+  </si>
+  <si>
+    <t>5.19</t>
+  </si>
+  <si>
+    <t>5.20</t>
+  </si>
+  <si>
+    <t>5.21</t>
+  </si>
+  <si>
+    <t>5.22</t>
+  </si>
+  <si>
+    <t>5.23</t>
+  </si>
+  <si>
+    <t>5.24</t>
+  </si>
+  <si>
+    <t>5.25</t>
+  </si>
+  <si>
+    <t>5.26</t>
+  </si>
+  <si>
+    <t>5.27</t>
+  </si>
+  <si>
+    <t>5.28</t>
+  </si>
+  <si>
+    <t>5.29</t>
+  </si>
+  <si>
+    <t>termodinamica</t>
+  </si>
+  <si>
+    <t>6.1</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>6.3</t>
+  </si>
+  <si>
+    <t>6.4</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>6.7</t>
+  </si>
+  <si>
+    <t>6.8</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>6.10</t>
+  </si>
+  <si>
+    <t>6.11</t>
+  </si>
+  <si>
+    <t>6.12</t>
+  </si>
+  <si>
+    <t>6.13</t>
+  </si>
+  <si>
+    <t>6.14</t>
+  </si>
+  <si>
+    <t>6.15</t>
+  </si>
+  <si>
+    <t>6.16</t>
+  </si>
+  <si>
+    <t>6.17</t>
+  </si>
+  <si>
+    <t>6.18</t>
+  </si>
+  <si>
+    <t>6.19</t>
+  </si>
+  <si>
+    <t>6.20</t>
+  </si>
+  <si>
+    <t>6.21</t>
+  </si>
+  <si>
+    <t>6.22</t>
+  </si>
+  <si>
+    <t>6.23</t>
   </si>
 </sst>
 </file>
@@ -273,7 +435,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -281,28 +443,32 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFFF0000"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -634,20 +800,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DA71AA-2E3E-4067-A12B-8A0B906B382C}">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="10" max="10" width="22.21875" customWidth="1"/>
+    <col min="13" max="13" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -657,8 +825,14 @@
       <c r="G1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>73</v>
+      </c>
+      <c r="M1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -674,8 +848,14 @@
       <c r="G3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -691,8 +871,14 @@
       <c r="G4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -708,8 +894,14 @@
       <c r="G5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J5" t="s">
+        <v>76</v>
+      </c>
+      <c r="M5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -722,8 +914,14 @@
       <c r="G6" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J6" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -736,8 +934,14 @@
       <c r="G7" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J7" t="s">
+        <v>78</v>
+      </c>
+      <c r="M7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -750,8 +954,14 @@
       <c r="G8" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -764,8 +974,14 @@
       <c r="G9" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -781,8 +997,14 @@
       <c r="G10" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J10" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -795,8 +1017,14 @@
       <c r="G11" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J11" t="s">
+        <v>82</v>
+      </c>
+      <c r="M11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -809,8 +1037,14 @@
       <c r="G12" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -823,8 +1057,14 @@
       <c r="G13" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J13" t="s">
+        <v>84</v>
+      </c>
+      <c r="M13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -834,14 +1074,20 @@
       <c r="D14" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" t="s">
         <v>25</v>
       </c>
       <c r="G14" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J14" t="s">
+        <v>85</v>
+      </c>
+      <c r="M14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -851,8 +1097,14 @@
       <c r="G15" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J15" t="s">
+        <v>86</v>
+      </c>
+      <c r="M15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -862,8 +1114,14 @@
       <c r="G16" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16" t="s">
+        <v>87</v>
+      </c>
+      <c r="M16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -873,8 +1131,14 @@
       <c r="G17" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17" t="s">
+        <v>88</v>
+      </c>
+      <c r="M17" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -884,8 +1148,14 @@
       <c r="G18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18" t="s">
+        <v>89</v>
+      </c>
+      <c r="M18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -895,8 +1165,14 @@
       <c r="G19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19" t="s">
+        <v>90</v>
+      </c>
+      <c r="M19" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -906,8 +1182,14 @@
       <c r="G20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J20" t="s">
+        <v>91</v>
+      </c>
+      <c r="M20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -917,8 +1199,14 @@
       <c r="G21" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J21" t="s">
+        <v>92</v>
+      </c>
+      <c r="M21" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -928,8 +1216,14 @@
       <c r="G22" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" t="s">
+        <v>93</v>
+      </c>
+      <c r="M22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -939,8 +1233,14 @@
       <c r="G23" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J23" t="s">
+        <v>94</v>
+      </c>
+      <c r="M23" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -950,35 +1250,85 @@
       <c r="G24" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
+        <v>95</v>
+      </c>
+      <c r="M24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="D25" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>96</v>
+      </c>
+      <c r="M25" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
+      <c r="J26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A3:A26 G3:G24 D18:D25 D3:D7 D10:D15 E3:E5 E10 E14">
-    <cfRule type="expression" dxfId="2" priority="1">
+  <conditionalFormatting sqref="A3:A26 G3:G24 D18:D25 D3:D7 D10:D15 E3:E5 E10 E14 H3">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>B3="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D17">
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>E8="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D8:D9">
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>#REF!="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J31">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>K3="x"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3:M25">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>N3="x"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>